<commit_message>
updated batch additional test scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelDataInput.xlsx
+++ b/src/main/resources/ExcelDataInput.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaniknadan/git/phase2lmsapihackathon/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\phase2lmsapihackathon\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F6370B-42F7-D54E-B9C4-E991C78B52A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD39DA0-D800-492B-8273-2175A5F66DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40440" yWindow="6280" windowWidth="37520" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getBatch" sheetId="3" r:id="rId1"/>
-    <sheet name="getBatchById" sheetId="4" r:id="rId2"/>
-    <sheet name="getBatchByName" sheetId="5" r:id="rId3"/>
-    <sheet name="postBatch" sheetId="2" r:id="rId4"/>
+    <sheet name="getBatchByProgramId" sheetId="6" r:id="rId2"/>
+    <sheet name="updateByBatchId" sheetId="7" r:id="rId3"/>
+    <sheet name="getBatchById" sheetId="4" r:id="rId4"/>
+    <sheet name="getBatchByName" sheetId="5" r:id="rId5"/>
+    <sheet name="postBatch" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="74">
   <si>
     <t>batchName</t>
   </si>
@@ -188,6 +190,75 @@
   </si>
   <si>
     <t>DA 05</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>/batches/program/</t>
+  </si>
+  <si>
+    <t>/batches/programxyz/</t>
+  </si>
+  <si>
+    <t>16306</t>
+  </si>
+  <si>
+    <t>9834958743</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>/batches/</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>Evening Batch</t>
+  </si>
+  <si>
+    <t>Morning Batch</t>
+  </si>
+  <si>
+    <t>API Icons</t>
+  </si>
+  <si>
+    <t>RestAssured Icons</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>SoftwareTesting525</t>
+  </si>
+  <si>
+    <t>SoftwareTesting524</t>
+  </si>
+  <si>
+    <t>SoftwareTesting523</t>
+  </si>
+  <si>
+    <t>first sdet</t>
+  </si>
+  <si>
+    <t>MAR24-APITrooper-SDET-Updated-115</t>
+  </si>
+  <si>
+    <t>400-  Bad Request</t>
+  </si>
+  <si>
+    <t>first sdet 123</t>
+  </si>
+  <si>
+    <t>/batches1243123/</t>
+  </si>
+  <si>
+    <t>17454adsd</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -229,9 +300,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,9 +322,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -290,7 +362,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -396,7 +468,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -538,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,15 +621,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E1" sqref="E1:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -626,6 +698,642 @@
       </c>
       <c r="E4" t="s">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05536965-096A-42BF-A9D8-25EEC59AD925}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="59.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A66F74B-DE98-4428-B2F0-4492C7993B80}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="59.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2">
+        <v>17466</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="2">
+        <v>17465</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>17464</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <v>17458</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="2">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8486</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2">
+        <v>17465</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="2">
+        <v>8486</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <v>17454</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="2">
+        <v>8486</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="2">
+        <v>17458</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2">
+        <v>8566</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17A3800-C5B4-044A-BFA7-92D0D1CD0E37}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="59.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -634,147 +1342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17A3800-C5B4-044A-BFA7-92D0D1CD0E37}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41397A5-BCA5-4745-8E36-D569E46812E7}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -782,10 +1350,10 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -914,7 +1482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -922,12 +1490,12 @@
       <selection activeCell="C17" sqref="C17:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1034,4 +1602,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>